<commit_message>
First batch of revisions for my thesis
</commit_message>
<xml_diff>
--- a/spreadsheets/Lab scale experiment_TS reduction.xlsx
+++ b/spreadsheets/Lab scale experiment_TS reduction.xlsx
@@ -72,10 +72,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,9 +113,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -169,7 +181,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,11 +430,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="7646109"/>
-        <c:axId val="26432608"/>
+        <c:axId val="21236686"/>
+        <c:axId val="74999178"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7646109"/>
+        <c:axId val="21236686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,12 +476,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26432608"/>
+        <c:crossAx val="74999178"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26432608"/>
+        <c:axId val="74999178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +523,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7646109"/>
+        <c:crossAx val="21236686"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -710,11 +722,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="29525397"/>
-        <c:axId val="78542232"/>
+        <c:axId val="95531123"/>
+        <c:axId val="94049618"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29525397"/>
+        <c:axId val="95531123"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,12 +768,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78542232"/>
+        <c:crossAx val="94049618"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78542232"/>
+        <c:axId val="94049618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +815,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29525397"/>
+        <c:crossAx val="95531123"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -857,7 +869,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Water reduction (g)</a:t>
+              <a:t>Water reduction plot</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1003,11 +1015,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45206978"/>
-        <c:axId val="63432348"/>
+        <c:axId val="183248"/>
+        <c:axId val="12909475"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45206978"/>
+        <c:axId val="183248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,6 +1035,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time (days)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1049,12 +1089,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63432348"/>
+        <c:crossAx val="12909475"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63432348"/>
+        <c:axId val="12909475"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,6 +1110,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Water Reduction (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1096,7 +1164,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45206978"/>
+        <c:crossAx val="183248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1295,11 +1363,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33593617"/>
-        <c:axId val="91318594"/>
+        <c:axId val="7535519"/>
+        <c:axId val="80408273"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33593617"/>
+        <c:axId val="7535519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,12 +1409,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91318594"/>
+        <c:crossAx val="80408273"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91318594"/>
+        <c:axId val="80408273"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1456,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33593617"/>
+        <c:crossAx val="7535519"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1587,11 +1655,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="12610469"/>
-        <c:axId val="57686344"/>
+        <c:axId val="28553877"/>
+        <c:axId val="83617289"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12610469"/>
+        <c:axId val="28553877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,12 +1701,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57686344"/>
+        <c:crossAx val="83617289"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57686344"/>
+        <c:axId val="83617289"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1748,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12610469"/>
+        <c:crossAx val="28553877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1719,9 +1787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>846360</xdr:colOff>
+      <xdr:colOff>846000</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1730,7 +1798,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9630360" y="1956960"/>
-        <a:ext cx="5452560" cy="2742840"/>
+        <a:ext cx="5452200" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1749,9 +1817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>888480</xdr:colOff>
+      <xdr:colOff>888120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1760,7 +1828,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3972240" y="1968480"/>
-        <a:ext cx="5181480" cy="2742840"/>
+        <a:ext cx="5181120" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1773,15 +1841,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>136080</xdr:colOff>
+      <xdr:colOff>140760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>424440</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>283320</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1789,8 +1857,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15591240" y="2122920"/>
-        <a:ext cx="5204520" cy="2742840"/>
+        <a:off x="15595920" y="2117880"/>
+        <a:ext cx="5761080" cy="3137760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1809,9 +1877,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>700920</xdr:colOff>
+      <xdr:colOff>700560</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1820,7 +1888,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9503280" y="5079960"/>
-        <a:ext cx="5434200" cy="2743200"/>
+        <a:ext cx="5433840" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1839,9 +1907,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>608040</xdr:colOff>
+      <xdr:colOff>607680</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1850,7 +1918,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3691800" y="4968720"/>
-        <a:ext cx="5181480" cy="2743200"/>
+        <a:ext cx="5181120" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2042,8 +2110,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T35" activeCellId="0" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2612,7 +2680,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T35 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>